<commit_message>
emptied device key list
</commit_message>
<xml_diff>
--- a/backend/api/management/commands/api_devicekey.xlsx
+++ b/backend/api/management/commands/api_devicekey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbao/Documents/github/boardingpass/backend/api/management/commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{283EA74F-B674-2E49-8717-3B2BB4515F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D34F9E-F8E1-E541-87CC-FB0BF77911A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api_devicekey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>dev_eui</t>
   </si>
@@ -36,119 +36,11 @@
   <si>
     <t>organization_id</t>
   </si>
-  <si>
-    <t>claimed</t>
-  </si>
-  <si>
-    <t>A84041F7D184ED74</t>
-  </si>
-  <si>
-    <t>A840410000000100</t>
-  </si>
-  <si>
-    <t>E3AB3C9B3D7CB66E4B7ECAD8171B694D</t>
-  </si>
-  <si>
-    <t>A8404111C184ED75</t>
-  </si>
-  <si>
-    <t>FADFC4BA3D628EF4CBD44568649CA997</t>
-  </si>
-  <si>
-    <t>A84041D9F184ED76</t>
-  </si>
-  <si>
-    <t>72FD64A2CF92ADCF3D63B9B26B854ECF</t>
-  </si>
-  <si>
-    <t>A84041298184ED77</t>
-  </si>
-  <si>
-    <t>D3FAE4D876EFE299E7BC8D8856F793A2</t>
-  </si>
-  <si>
-    <t>A84041916184ED78</t>
-  </si>
-  <si>
-    <t>6999F5A8E5B9952CB6952988588FEF5A</t>
-  </si>
-  <si>
-    <t>A84041DD6184ED79</t>
-  </si>
-  <si>
-    <t>ED2A745F2854E4BA5DC112D982C82CB3</t>
-  </si>
-  <si>
-    <t>A84041C43184ED7A</t>
-  </si>
-  <si>
-    <t>4CB426D843DBC9969FDB9BE56BAD932A</t>
-  </si>
-  <si>
-    <t>A84041F5B184ED7B</t>
-  </si>
-  <si>
-    <t>9813C641742C36B627BAE4E197583ED7</t>
-  </si>
-  <si>
-    <t>A840415A7184ED7C</t>
-  </si>
-  <si>
-    <t>1E84A8F626FDEDE81F6966CA1A2EDBC3</t>
-  </si>
-  <si>
-    <t>A840419A2184ED7D</t>
-  </si>
-  <si>
-    <t>F6BE83B871A854D6EC68B8766ED2C8F4</t>
-  </si>
-  <si>
-    <t>A84041B33184ED7E</t>
-  </si>
-  <si>
-    <t>563C38D4C1894A2FCDD9841827EABDDE</t>
-  </si>
-  <si>
-    <t>A8404149F184ED7F</t>
-  </si>
-  <si>
-    <t>EB2F5A5E2D8DD225FBB5E219AFD446C9</t>
-  </si>
-  <si>
-    <t>A840414F7184ED80</t>
-  </si>
-  <si>
-    <t>4E7BF1F9345ACAF6EFEAAD4B8FAD7D9C</t>
-  </si>
-  <si>
-    <t>A84041B72184ED81</t>
-  </si>
-  <si>
-    <t>C4F43A839417F491C5493895C78BBC65</t>
-  </si>
-  <si>
-    <t>A840418E2184ED82</t>
-  </si>
-  <si>
-    <t>F7926E826A287AE729D48329BA7DCE32</t>
-  </si>
-  <si>
-    <t>A8404197C184ED83</t>
-  </si>
-  <si>
-    <t>14A9212BB8FFBCE22EF3EF745963A83A</t>
-  </si>
-  <si>
-    <t>A84041E8F184ED84</t>
-  </si>
-  <si>
-    <t>38558A9ED31EC99AAEA344C7772AC6A3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -989,11 +881,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E18" sqref="A2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,293 +911,89 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>